<commit_message>
Update inflow variable data conversion
</commit_message>
<xml_diff>
--- a/scripting/variables_checklist/initial_values.xlsx
+++ b/scripting/variables_checklist/initial_values.xlsx
@@ -5,22 +5,36 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvette/Desktop/Work/UWA AED/Hydro Tasmania/tassie-lake/tassielakes-data/scripting/variables_checklist/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvette/Desktop/Work/UWA AED/Hydro Tasmania/updates/tassielakes-data/scripting/variables_checklist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D1A5704E-F6C3-5841-B8A2-3CCFBE20AAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BC4156D9-67C3-F34D-90A3-23A51B1E4571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" xr2:uid="{A915CF26-A3D2-AF47-BE91-8BF95CB6824A}"/>
   </bookViews>
   <sheets>
-    <sheet name="initial_values" sheetId="1" r:id="rId1"/>
+    <sheet name="model" sheetId="3" r:id="rId1"/>
+    <sheet name="initial_values" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="108">
   <si>
     <t>Variable</t>
   </si>
@@ -338,13 +352,19 @@
   </si>
   <si>
     <t>not available in TFV data</t>
+  </si>
+  <si>
+    <t>Initial Value (TFV unit)</t>
+  </si>
+  <si>
+    <t>Conversion factor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -486,6 +506,13 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -674,7 +701,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -851,6 +878,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -896,7 +932,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -908,6 +944,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1282,11 +1321,291 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7D4D684-DFF7-F045-82C8-EFDD92D3A02D}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="50.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="11" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="11">
+        <v>2.7958E-2</v>
+      </c>
+      <c r="C2" s="11">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="11">
+        <f>B2*C2</f>
+        <v>2.7958E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="12">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="11">
+        <f t="shared" ref="E3:E14" si="0">B3*C3</f>
+        <v>88.283496999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="11">
+        <v>99.3</v>
+      </c>
+      <c r="C4" s="11">
+        <v>1</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="11">
+        <f t="shared" si="0"/>
+        <v>99.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="11">
+        <v>36.950000000000003</v>
+      </c>
+      <c r="C5" s="11">
+        <v>1</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="11">
+        <f t="shared" si="0"/>
+        <v>36.950000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="11">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="C6" s="11">
+        <f>1000/14</f>
+        <v>71.428571428571431</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="11">
+        <f t="shared" si="0"/>
+        <v>60.357142857142854</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="12">
+        <f>1000/31</f>
+        <v>32.258064516129032</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="11">
+        <f t="shared" si="0"/>
+        <v>0.83870967741935476</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="11">
+        <v>8</v>
+      </c>
+      <c r="C8" s="11">
+        <v>1</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="11">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="11">
+        <v>17.925000000000001</v>
+      </c>
+      <c r="C9" s="11">
+        <v>1</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="11">
+        <f t="shared" si="0"/>
+        <v>17.925000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C10" s="11">
+        <f>1000/14</f>
+        <v>71.428571428571431</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" si="0"/>
+        <v>0.35714285714285715</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11" s="11">
+        <f>1000/14</f>
+        <v>71.428571428571431</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="11">
+        <f t="shared" si="0"/>
+        <v>0.35714285714285715</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="11">
+        <v>7.15</v>
+      </c>
+      <c r="C12" s="11">
+        <v>83.333332999999996</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="11">
+        <f t="shared" si="0"/>
+        <v>595.83333095</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="11">
+        <v>9.0759924999999999</v>
+      </c>
+      <c r="C13" s="11">
+        <f>1000/32</f>
+        <v>31.25</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" s="11">
+        <f t="shared" si="0"/>
+        <v>283.62476562500001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C14" s="11">
+        <f>1000/32</f>
+        <v>31.25</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="11">
+        <f t="shared" si="0"/>
+        <v>0.15625</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736A9200-9DDC-034F-9CAB-6238B037B27F}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="92" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView zoomScale="92" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Python plots on variables in marvl aed plot, extract median value for each variable within plotting period
</commit_message>
<xml_diff>
--- a/scripting/variables_checklist/initial_values.xlsx
+++ b/scripting/variables_checklist/initial_values.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yvette/Desktop/Work/UWA AED/Hydro Tasmania/updates/tassielakes-data/scripting/variables_checklist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1B3322D8-12AB-2941-B69E-759986962C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E428EA6-F526-F346-93F0-59A3908118DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17200" xr2:uid="{A915CF26-A3D2-AF47-BE91-8BF95CB6824A}"/>
   </bookViews>
   <sheets>
-    <sheet name="model" sheetId="3" r:id="rId1"/>
-    <sheet name="initial_values" sheetId="1" r:id="rId2"/>
+    <sheet name="model_medianDataModelAvailable" sheetId="4" r:id="rId1"/>
+    <sheet name="model_medianDateBeforeAfter" sheetId="3" r:id="rId2"/>
+    <sheet name="initial_values" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="110">
   <si>
     <t>Variable</t>
   </si>
@@ -358,6 +359,12 @@
   </si>
   <si>
     <t>Conversion factor</t>
+  </si>
+  <si>
+    <t>TEMP</t>
+  </si>
+  <si>
+    <t>WoodsLakeMiddleLakeContinuous_Temperature</t>
   </si>
 </sst>
 </file>
@@ -944,9 +951,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1321,278 +1328,350 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7D4D684-DFF7-F045-82C8-EFDD92D3A02D}">
-  <dimension ref="A1:E14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF5043B7-BECF-4945-8EE7-63FEE49D1875}">
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5" style="11" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" style="11" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="11"/>
+    <col min="1" max="1" width="50.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="11">
-        <v>2.7958E-2</v>
-      </c>
-      <c r="C2" s="11">
+      <c r="B2" s="12">
+        <v>2.76E-2</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2">
         <f>B2*C2</f>
-        <v>2.7958E-2</v>
+        <v>2.76E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="12">
+      <c r="B3" s="13">
+        <v>87.946600000000004</v>
+      </c>
+      <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="11">
-        <f t="shared" ref="E3:E14" si="0">B3*C3</f>
-        <v>88.283496999999997</v>
+      <c r="E3">
+        <f t="shared" ref="E3:E16" si="0">B3*C3</f>
+        <v>87.946600000000004</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="12">
         <v>99.3</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4">
         <f t="shared" si="0"/>
         <v>99.3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+      <c r="A5" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="11">
-        <v>36.950000000000003</v>
-      </c>
-      <c r="C5" s="11">
+      <c r="B5" s="12">
+        <v>30.5</v>
+      </c>
+      <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5">
         <f t="shared" si="0"/>
-        <v>36.950000000000003</v>
+        <v>30.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="11">
-        <v>0.84499999999999997</v>
-      </c>
-      <c r="C6" s="11">
+      <c r="B6" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="C6">
         <f>1000/14</f>
         <v>71.428571428571431</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6">
         <f t="shared" si="0"/>
-        <v>60.357142857142854</v>
+        <v>107.14285714285714</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="A7" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="12">
+      <c r="B7" s="13">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="C7" s="1">
         <f>1000/31</f>
         <v>32.258064516129032</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7">
         <f t="shared" si="0"/>
-        <v>0.83870967741935476</v>
+        <v>1.064516129032258</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="A8" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="11">
-        <v>8</v>
-      </c>
-      <c r="C8" s="11">
+      <c r="B8" s="12">
+        <v>12</v>
+      </c>
+      <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="A9" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="11">
-        <v>17.925000000000001</v>
-      </c>
-      <c r="C9" s="11">
+      <c r="B9" s="12">
+        <v>16</v>
+      </c>
+      <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9">
         <f t="shared" si="0"/>
-        <v>17.925000000000001</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="12">
+        <v>21.985199999999999</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>21.985199999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B11" s="12">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C11">
         <f>1000/14</f>
         <v>71.428571428571431</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D11" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E11">
         <f t="shared" si="0"/>
         <v>0.35714285714285715</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="11">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C11" s="11">
+      <c r="B12" s="12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="C12">
         <f>1000/14</f>
         <v>71.428571428571431</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D12" t="s">
         <v>83</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E12">
         <f t="shared" si="0"/>
-        <v>0.35714285714285715</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
+        <v>1.2857142857142856</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="11">
-        <v>7.15</v>
-      </c>
-      <c r="C12" s="11">
+      <c r="B13" s="12">
+        <v>11</v>
+      </c>
+      <c r="C13">
         <v>83.333332999999996</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D13" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E13">
         <f t="shared" si="0"/>
-        <v>595.83333095</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" s="11">
-        <v>9.0759924999999999</v>
-      </c>
-      <c r="C13" s="11">
+        <v>916.66666299999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="12">
+        <v>10.25</v>
+      </c>
+      <c r="C14">
         <f>1000/32</f>
         <v>31.25</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D14" t="s">
         <v>89</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E14">
         <f t="shared" si="0"/>
-        <v>283.62476562500001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="B14" s="11">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C14" s="11">
+        <v>320.3125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="12">
+        <v>8.6189999999999998</v>
+      </c>
+      <c r="C15">
         <f>1000/32</f>
         <v>31.25</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>269.34375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="12">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C16">
+        <f>1000/32</f>
+        <v>31.25</v>
+      </c>
+      <c r="D16" t="s">
         <v>92</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E16">
         <f t="shared" si="0"/>
-        <v>0.15625</v>
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="12">
+        <v>12.4</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17">
+        <f>B17*C17</f>
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="12">
+        <v>16.501799999999999</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18">
+        <f>B18*C18</f>
+        <v>16.501799999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1601,6 +1680,285 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7D4D684-DFF7-F045-82C8-EFDD92D3A02D}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="50.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>2.7958E-2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <f>B2*C2</f>
+        <v>2.7958E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E14" si="0">B3*C3</f>
+        <v>88.283496999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>99.3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>99.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5">
+        <v>36.950000000000003</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>36.950000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="C6">
+        <f>1000/14</f>
+        <v>71.428571428571431</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>60.357142857142854</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="1">
+        <f>1000/31</f>
+        <v>32.258064516129032</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.83870967741935476</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9">
+        <v>17.925000000000001</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>17.925000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C10">
+        <f>1000/14</f>
+        <v>71.428571428571431</v>
+      </c>
+      <c r="D10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.35714285714285715</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <f>1000/14</f>
+        <v>71.428571428571431</v>
+      </c>
+      <c r="D11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.35714285714285715</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12">
+        <v>7.15</v>
+      </c>
+      <c r="C12">
+        <v>83.333332999999996</v>
+      </c>
+      <c r="D12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>595.83333095</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13">
+        <v>9.0759924999999999</v>
+      </c>
+      <c r="C13">
+        <f>1000/32</f>
+        <v>31.25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>283.62476562500001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C14">
+        <f>1000/32</f>
+        <v>31.25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.15625</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736A9200-9DDC-034F-9CAB-6238B037B27F}">
   <dimension ref="A1:G51"/>
   <sheetViews>

</xml_diff>